<commit_message>
Revisión de la Primera historia de Usuario
Me encargaré de hacer los prototipos con el mockup
</commit_message>
<xml_diff>
--- a/Requerimientos/Backlog _J&G.xlsx
+++ b/Requerimientos/Backlog _J&G.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XxItz.D13g0xX\Documents\GitHub\evosoft\Requerimientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XxItz.D13g0xX\Documents\GitHub\evosoft\Gestion_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -250,7 +250,13 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -270,12 +276,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,7 +562,7 @@
   <dimension ref="A2:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,563 +587,563 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
     </row>
     <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="14" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="14" t="s">
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="13" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="7" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="13" t="s">
+      <c r="I7" s="10"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="13" t="s">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="5" t="s">
+      <c r="J8" s="4"/>
+      <c r="K8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="5" t="s">
+      <c r="P8" s="4"/>
+      <c r="Q8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T8" s="5" t="s">
+      <c r="T8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="U8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>0.1</v>
       </c>
       <c r="E9">
         <v>15</v>
       </c>
       <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H9" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12">
+      <c r="K9" s="14"/>
+      <c r="L9" s="14">
         <v>10</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="14">
         <v>15</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="14">
         <v>20</v>
       </c>
-      <c r="O9" s="12">
+      <c r="O9" s="14">
         <v>16</v>
       </c>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12">
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14">
         <v>9</v>
       </c>
-      <c r="S9" s="12">
+      <c r="S9" s="14">
         <v>8</v>
       </c>
-      <c r="T9" s="12">
+      <c r="T9" s="14">
         <v>0</v>
       </c>
-      <c r="U9" s="12">
+      <c r="U9" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>0.15</v>
       </c>
       <c r="E10">
         <v>13</v>
       </c>
       <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>40</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12">
+      <c r="K10" s="14"/>
+      <c r="L10" s="14">
         <v>9</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="14">
         <v>14</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="14">
         <v>18</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="14">
         <v>14</v>
       </c>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12">
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14">
         <v>8</v>
       </c>
-      <c r="S10" s="12">
+      <c r="S10" s="14">
         <v>8</v>
       </c>
-      <c r="T10" s="12">
+      <c r="T10" s="14">
         <v>0</v>
       </c>
-      <c r="U10" s="12">
+      <c r="U10" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>0.11</v>
       </c>
       <c r="E11">
         <v>13</v>
       </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>48</v>
       </c>
       <c r="H11" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E12">
         <v>14</v>
       </c>
       <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>40</v>
       </c>
       <c r="H12" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12">
+      <c r="K12" s="14"/>
+      <c r="L12" s="14">
         <v>14</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M12" s="14">
         <v>18</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="14">
         <v>22</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="14">
         <v>16</v>
       </c>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12">
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14">
         <v>6</v>
       </c>
-      <c r="S12" s="12">
+      <c r="S12" s="14">
         <v>5</v>
       </c>
-      <c r="T12" s="12">
+      <c r="T12" s="14">
         <v>0</v>
       </c>
-      <c r="U12" s="12">
+      <c r="U12" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>0.1</v>
       </c>
       <c r="E13">
         <v>13</v>
       </c>
       <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>40</v>
       </c>
       <c r="H13" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12">
+      <c r="K13" s="14"/>
+      <c r="L13" s="14">
         <v>11</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M13" s="14">
         <v>17</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="14">
         <v>21</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="14">
         <v>16</v>
       </c>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12">
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14">
         <v>11</v>
       </c>
-      <c r="S13" s="12">
+      <c r="S13" s="14">
         <v>14</v>
       </c>
-      <c r="T13" s="12">
+      <c r="T13" s="14">
         <v>0</v>
       </c>
-      <c r="U13" s="12">
+      <c r="U13" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>0.15</v>
       </c>
       <c r="E14">
         <v>13</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="13" t="s">
         <v>41</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>0.11</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H15" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>0.11</v>
       </c>
       <c r="E16">
         <v>13</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H16" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>0.1</v>
       </c>
       <c r="E17">
         <v>13</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H17" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="G18" s="10"/>
+      <c r="C18" s="2"/>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="10"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G20" s="10"/>
+      <c r="G20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>